<commit_message>
vamstudio : add status json sample
</commit_message>
<xml_diff>
--- a/ref/doc/dev_contents-admin.xlsx
+++ b/ref/doc/dev_contents-admin.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\2018\2018_0412_LAB\01_Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\2018\2018_0718_Workgroup_DF\git\work-group\ref\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31090" windowHeight="17240" tabRatio="738"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31090" windowHeight="17240" tabRatio="738" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="컨텐츠 리스트" sheetId="1" r:id="rId1"/>
-    <sheet name="컨텐츠 등록-수정" sheetId="2" r:id="rId2"/>
-    <sheet name="콘텐츠 운영" sheetId="3" r:id="rId3"/>
+    <sheet name="배경 컨텐츠 리스트" sheetId="1" r:id="rId1"/>
+    <sheet name="배경 컨텐츠 등록(&amp;수정)" sheetId="2" r:id="rId2"/>
+    <sheet name="일정,공지 리스트" sheetId="3" r:id="rId3"/>
+    <sheet name="일정 등록하기" sheetId="4" r:id="rId4"/>
+    <sheet name="공지 등록하기" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="159">
   <si>
     <t>bg database</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -557,6 +559,110 @@
   </si>
   <si>
     <t>1080*1920(모바일용 이미지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정 등록하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018 08 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(date)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드랍다운 메뉴로 선택(기본:04)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트로 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜 선택(기본:내일날짜)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; 일정 등록하기 &gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>line 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>line 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>line 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닥 세미나가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한줄에 최대 7자까지 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한줄에 최대 20자까지 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오후 4시까지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지하1층 바닥 세미나실로 모여주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 경영지원팀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; 공지 등록하기 &gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지 등록하기(수정)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -885,7 +991,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1014,6 +1120,36 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1297,7 +1433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -2005,7 +2141,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:E49"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2741,52 +2877,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.4140625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="15.58203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.4140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.9140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.9140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="3.4140625" style="1" customWidth="1"/>
-    <col min="12" max="15" width="15.58203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="3.4140625" style="1" customWidth="1"/>
+    <col min="3" max="6" width="15.58203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.4140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.9140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.9140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3.4140625" style="1" customWidth="1"/>
+    <col min="13" max="16" width="15.58203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9">
+    <row r="1" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9">
         <v>2018</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>2017</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="10"/>
-      <c r="B4" s="16" t="s">
+    <row r="3" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B4" s="10"/>
+      <c r="C4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -2794,224 +2930,224 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="10"/>
-      <c r="B5" s="15" t="s">
+      <c r="K4" s="14"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B5" s="10"/>
+      <c r="C5" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="I5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="15"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="10"/>
-      <c r="B6" s="5" t="s">
+      <c r="K5" s="15"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B6" s="10"/>
+      <c r="C6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="10"/>
-      <c r="B7" s="5" t="s">
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B7" s="10"/>
+      <c r="C7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="10"/>
-      <c r="B8" s="5" t="s">
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B8" s="10"/>
+      <c r="C8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="10"/>
-      <c r="B9" s="5" t="s">
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B9" s="10"/>
+      <c r="C9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="11"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" s="10"/>
-      <c r="B10" s="5" t="s">
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B10" s="10"/>
+      <c r="C10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="10"/>
-      <c r="B11" s="5" t="s">
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B11" s="10"/>
+      <c r="C11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="1:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="12"/>
-      <c r="B12" s="17"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="12"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -3020,15 +3156,18 @@
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" s="10"/>
-      <c r="B14" s="16" t="s">
+      <c r="K12" s="17"/>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -3036,182 +3175,190 @@
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15" s="10"/>
-      <c r="B15" s="15" t="s">
+      <c r="K14" s="14"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="19"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="E15" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="11"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" s="10"/>
-      <c r="B16" s="5" t="s">
+      <c r="K15" s="15"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="19"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5"/>
+      <c r="J16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="K16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17" s="10"/>
-      <c r="B17" s="5" t="s">
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="19"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="5"/>
+      <c r="J17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="K17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="11"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18" s="10"/>
-      <c r="B18" s="5" t="s">
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="19"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5"/>
+      <c r="J18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="K18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K18" s="11"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A19" s="10"/>
-      <c r="B19" s="5" t="s">
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="19"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="5"/>
+      <c r="J19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A20" s="10"/>
-      <c r="B20" s="5" t="s">
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="19"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="5"/>
+      <c r="G20" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5"/>
+      <c r="J20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="K20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K20" s="11"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A21" s="10"/>
-      <c r="B21" s="5" t="s">
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="19"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="5"/>
+      <c r="G21" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5"/>
+      <c r="J21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="K21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K21" s="11"/>
-    </row>
-    <row r="22" spans="1:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="12"/>
-      <c r="B22" s="17"/>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="19"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -3220,7 +3367,274 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
-      <c r="K22" s="13"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="13"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B1" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B7" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C9" s="43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.08203125" customWidth="1"/>
+    <col min="5" max="5" width="26.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="19"/>
+      <c r="B3" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="19"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="47"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="19"/>
+      <c r="B5" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="19"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="19"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="19"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="44"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="19"/>
+      <c r="B9" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="19"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="19"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="19"/>
+      <c r="C13" s="43" t="s">
+        <v>158</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>